<commit_message>
- code fix to ensure execution metadata is generated when `nexial.outputToCloud` is set to true. This is needed to   update Execution Dashboard.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/jmeter-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/jmeter-showcase.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBE844B-44D8-6D4F-9412-56B0ECC12D28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF339D2B-FBD9-3E4F-9405-A570628FBD2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34140" yWindow="440" windowWidth="17060" windowHeight="31560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
   <si>
     <t>true</t>
   </si>
@@ -171,9 +171,6 @@
     <t>(empty)</t>
   </si>
   <si>
-    <t>\$\{(?!__P\)[0-9A-Za-z_\-\.\,]+\}</t>
-  </si>
-  <si>
     <t>testname/Regex 1</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>variable/returnVar</t>
   </si>
   <si>
-    <t>variable/sleepTime</t>
-  </si>
-  <si>
     <t>snr.configFile</t>
   </si>
   <si>
@@ -376,6 +370,18 @@
   </si>
   <si>
     <t>testname/For 1</t>
+  </si>
+  <si>
+    <t>\$\{(?!__P\)[0-9A-Za-z_\-\.\,\ \/\\]+\}</t>
+  </si>
+  <si>
+    <t>variable/sleep time</t>
+  </si>
+  <si>
+    <t>c'mon back</t>
+  </si>
+  <si>
+    <t>spaces and slashes \\ / = . \, !@#\$%^&amp;</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1178,7 @@
   <dimension ref="A1:AAA39"/>
   <sheetViews>
     <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1276,7 +1282,7 @@
     </row>
     <row r="10" spans="1:703" ht="22" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -1286,7 +1292,7 @@
     </row>
     <row r="11" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A11" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>3</v>
@@ -1299,7 +1305,7 @@
     </row>
     <row r="12" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A12" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
@@ -1311,7 +1317,7 @@
     </row>
     <row r="13" spans="1:703" ht="22" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>14</v>
@@ -1324,10 +1330,10 @@
     </row>
     <row r="14" spans="1:703" ht="22" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -1360,7 +1366,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1370,10 +1376,10 @@
     </row>
     <row r="18" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A18" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1383,7 +1389,7 @@
     </row>
     <row r="19" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A19" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
@@ -1404,10 +1410,10 @@
     </row>
     <row r="21" spans="1:703" ht="22" customHeight="1">
       <c r="A21" s="23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -1415,10 +1421,10 @@
     </row>
     <row r="22" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>25</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -1426,7 +1432,7 @@
     </row>
     <row r="23" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A23" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
@@ -1436,10 +1442,10 @@
     </row>
     <row r="24" spans="1:703" ht="22" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -1447,10 +1453,10 @@
     </row>
     <row r="25" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1458,7 +1464,7 @@
     </row>
     <row r="26" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A26" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1468,10 +1474,10 @@
     </row>
     <row r="27" spans="1:703" ht="22" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -1479,10 +1485,10 @@
     </row>
     <row r="28" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A28" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1490,7 +1496,7 @@
     </row>
     <row r="29" spans="1:703" ht="22" customHeight="1" thickBot="1">
       <c r="A29" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
@@ -1500,10 +1506,10 @@
     </row>
     <row r="30" spans="1:703" ht="22" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -1511,74 +1517,74 @@
     </row>
     <row r="31" spans="1:703" ht="22" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:703" ht="22" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="22" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="22" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="22" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="22" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="22" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="22" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="22" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1610,7 +1616,7 @@
   <dimension ref="A1:AAA100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1624,7 +1630,7 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1">
       <c r="A1" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>22</v>
@@ -1634,7 +1640,7 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1644,7 +1650,7 @@
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -1664,7 +1670,7 @@
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -1674,7 +1680,7 @@
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
@@ -1684,7 +1690,7 @@
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
@@ -1694,7 +1700,7 @@
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
@@ -1704,7 +1710,7 @@
     </row>
     <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -1714,7 +1720,7 @@
     </row>
     <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
@@ -1722,7 +1728,7 @@
     </row>
     <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
@@ -1730,7 +1736,7 @@
     </row>
     <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
@@ -1738,7 +1744,7 @@
     </row>
     <row r="13" spans="1:703" ht="23" customHeight="1">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
@@ -1746,7 +1752,7 @@
     </row>
     <row r="14" spans="1:703" ht="23" customHeight="1">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
@@ -1754,7 +1760,7 @@
     </row>
     <row r="15" spans="1:703" ht="23" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1762,7 +1768,7 @@
     </row>
     <row r="16" spans="1:703" ht="23" customHeight="1">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
@@ -1770,7 +1776,7 @@
     </row>
     <row r="17" spans="1:2" ht="23" customHeight="1">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>0</v>
@@ -1778,7 +1784,7 @@
     </row>
     <row r="18" spans="1:2" ht="23" customHeight="1">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>0</v>
@@ -1786,7 +1792,7 @@
     </row>
     <row r="19" spans="1:2" ht="23" customHeight="1">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>0</v>
@@ -1794,7 +1800,7 @@
     </row>
     <row r="20" spans="1:2" ht="23" customHeight="1">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>200</v>
@@ -1802,42 +1808,42 @@
     </row>
     <row r="21" spans="1:2" ht="23" customHeight="1">
       <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21">
-        <v>300</v>
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="23" customHeight="1">
       <c r="A22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22">
-        <v>400</v>
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="23" customHeight="1">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="B23">
-        <v>500</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23" customHeight="1">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24">
-        <v>600</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="23" customHeight="1">
       <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="23" customHeight="1"/>

</xml_diff>